<commit_message>
Ajuste na criação da Zbus de sequencia zero
</commit_message>
<xml_diff>
--- a/data/exemplo_de_aula.xlsx
+++ b/data/exemplo_de_aula.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Nº</t>
   </si>
@@ -70,29 +70,20 @@
     <t>Xd</t>
   </si>
   <si>
+    <t>Xn</t>
+  </si>
+  <si>
     <t>Z0</t>
   </si>
   <si>
     <t>Zn</t>
-  </si>
-  <si>
-    <t>Ligação De</t>
-  </si>
-  <si>
-    <t>Ligação para</t>
-  </si>
-  <si>
-    <t>estrela</t>
-  </si>
-  <si>
-    <t>delta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -116,6 +107,10 @@
       <color theme="1"/>
       <name val="&quot;Times New Roman&quot;"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="&quot;Times New Roman&quot;"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -277,8 +272,8 @@
     <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
+    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -920,6 +915,12 @@
       <c r="C1" s="18" t="s">
         <v>17</v>
       </c>
+      <c r="D1" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="16">
@@ -928,6 +929,12 @@
       <c r="C2" s="16">
         <v>16.0</v>
       </c>
+      <c r="D2" s="16">
+        <v>0.04</v>
+      </c>
+      <c r="E2" s="16">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="16">
@@ -935,6 +942,12 @@
       </c>
       <c r="C3" s="16">
         <v>21.0</v>
+      </c>
+      <c r="D3" s="16">
+        <v>0.05</v>
+      </c>
+      <c r="E3" s="16">
+        <v>0.03</v>
       </c>
     </row>
   </sheetData>
@@ -980,16 +993,10 @@
         <v>13</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="19" t="s">
         <v>20</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3">
@@ -1008,14 +1015,8 @@
       <c r="F3" s="16">
         <v>0.45</v>
       </c>
-      <c r="G3" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>23</v>
+      <c r="G3" s="20">
+        <v>999999.0</v>
       </c>
     </row>
     <row r="4">
@@ -1034,14 +1035,8 @@
       <c r="F4" s="16">
         <v>0.3</v>
       </c>
-      <c r="G4" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>23</v>
+      <c r="G4" s="20">
+        <v>999999.0</v>
       </c>
     </row>
     <row r="5">
@@ -1060,14 +1055,8 @@
       <c r="F5" s="16">
         <v>0.35</v>
       </c>
-      <c r="G5" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="20" t="s">
-        <v>23</v>
+      <c r="G5" s="20">
+        <v>999999.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>